<commit_message>
checking issue for indication
</commit_message>
<xml_diff>
--- a/questions/Assignment5-BLEEventSchedulerGuidance.xlsx
+++ b/questions/Assignment5-BLEEventSchedulerGuidance.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiabinlin/SimplicityStudio/v5_workspace/ecen5823-assignment5-JiabinLin12/questions/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68583CBF-22C0-3643-82B9-ED2F950E4D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>A5 Command Table</t>
   </si>
@@ -157,20 +166,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="10"/>
@@ -178,13 +179,13 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -233,52 +234,38 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -288,24 +275,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff4d8f72"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF4D8F72"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -507,7 +555,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -526,7 +574,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -556,7 +604,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -582,7 +630,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -608,7 +656,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -634,7 +682,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -660,7 +708,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -686,7 +734,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -712,7 +760,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -738,7 +786,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -764,7 +812,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -777,9 +825,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -796,7 +850,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -815,7 +869,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -841,7 +895,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -867,7 +921,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -893,7 +947,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -919,7 +973,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -945,7 +999,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -971,7 +1025,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -997,7 +1051,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1023,7 +1077,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1049,7 +1103,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1062,9 +1116,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1078,7 +1138,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1097,7 +1157,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1127,7 +1187,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1153,7 +1213,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1179,7 +1239,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1205,7 +1265,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1231,7 +1291,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1257,7 +1317,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1283,7 +1343,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1309,7 +1369,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1335,7 +1395,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1348,395 +1408,405 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.0781" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7422" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.9844" style="1" customWidth="1"/>
-    <col min="4" max="5" width="33.9453" style="1" customWidth="1"/>
-    <col min="6" max="7" width="41.4688" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36" style="1" customWidth="1"/>
+    <col min="4" max="5" width="34" style="1" customWidth="1"/>
+    <col min="6" max="7" width="41.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="10.75" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="10.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" ht="13.1" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="14.35" customHeight="1">
-      <c r="A3" t="s" s="6">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" ht="50.35" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" t="s" s="6">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" t="s" s="6">
+      <c r="D4" s="8"/>
+      <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s" s="12">
+      <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="26.1" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" t="s" s="6">
+    <row r="5" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s" s="11">
+      <c r="F5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" ht="14.35" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" t="s" s="6">
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s" s="11">
+      <c r="F6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" ht="14.35" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" t="s" s="6">
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s" s="11">
+      <c r="F7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" ht="13.1" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" ht="39.1" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" t="s" s="6">
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s" s="11">
+      <c r="D9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s" s="6">
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F9" t="s" s="11">
+      <c r="F9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" ht="14.35" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" t="s" s="6">
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s" s="11">
+      <c r="F10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" ht="13.1" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" ht="26.35" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" t="s" s="6">
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s" s="13">
+      <c r="C12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s" s="11">
+      <c r="D12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s" s="6">
+      <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F12" t="s" s="11">
+      <c r="F12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" ht="13.1" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" ht="38.35" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" t="s" s="6">
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s" s="13">
+      <c r="C14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" ht="13.1" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" ht="38.35" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" t="s" s="6">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s" s="13">
+      <c r="C16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" ht="13.1" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" ht="14.35" customHeight="1">
-      <c r="A18" t="s" s="6">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" ht="74.35" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" t="s" s="6">
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C19" t="s" s="13">
+      <c r="C19" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D19" t="s" s="11">
+      <c r="D19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" ht="13.1" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" ht="50.35" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" t="s" s="6">
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C21" t="s" s="13">
+      <c r="C21" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D21" t="s" s="11">
+      <c r="D21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" ht="13.1" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" ht="12.9" customHeight="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" ht="12.9" customHeight="1">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" ht="12.9" customHeight="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" ht="12.9" customHeight="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" ht="12.9" customHeight="1">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" ht="12.9" customHeight="1">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" ht="12.9" customHeight="1">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" ht="12.9" customHeight="1">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>